<commit_message>
mit neuen imrana 2024 daten
</commit_message>
<xml_diff>
--- a/data/2024 Imrana-food/21_days.xlsx
+++ b/data/2024 Imrana-food/21_days.xlsx
@@ -38,7 +38,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,17 +51,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFffffff"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -71,35 +78,49 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
+      <left style="thin">
+        <color rgb="FFff0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFff0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFff0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFff0000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -129,10 +150,10 @@
         <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="4F818D"/>
@@ -406,149 +427,158 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
-        <v>87.5</v>
+      <c r="B2" s="5">
+        <v>88.3333333333333</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>21</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="G2" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="B3" s="4">
+        <v>1.66666666666667</v>
+      </c>
+      <c r="B3" s="5">
+        <v>96.6666666666667</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="4">
+        <v>3.33333333333333</v>
+      </c>
+      <c r="B4" s="5">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5">
+        <v>33.3333333333333</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="4">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5">
+        <v>93.3333333333333</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="4">
+        <v>33.3333333333333</v>
+      </c>
+      <c r="B6" s="5">
         <v>95</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="B4" s="4">
-        <v>87.5</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="4">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>92.5</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="4">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4">
-        <v>97.5</v>
-      </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="5">
-        <v>33</v>
-      </c>
-      <c r="B7" s="4">
-        <v>80</v>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="4">
+        <v>100</v>
+      </c>
+      <c r="B7" s="5">
+        <v>83.3333333333333</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="4">
-        <v>100</v>
-      </c>
-      <c r="B8" s="4">
-        <v>62.5</v>
+        <v>333.333333333333</v>
+      </c>
+      <c r="B8" s="5">
+        <v>55</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="4">
-        <v>330</v>
-      </c>
-      <c r="B9" s="4">
+        <v>1000</v>
+      </c>
+      <c r="B9" s="5">
         <v>0</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>